<commit_message>
Fixed Home Page Zip Test
</commit_message>
<xml_diff>
--- a/resources/web-data.xlsx
+++ b/resources/web-data.xlsx
@@ -24,9 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>ZIP</t>
+  </si>
+  <si>
+    <t>94538</t>
   </si>
 </sst>
 </file>
@@ -72,10 +75,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -360,7 +363,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -368,13 +373,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>94538</v>
+      <c r="A2" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>